<commit_message>
add comment column to excel data sheet
</commit_message>
<xml_diff>
--- a/src/SSDTHelperTest/TestData.xlsx
+++ b/src/SSDTHelperTest/TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="People" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>Age</t>
     <phoneticPr fontId="1"/>
@@ -100,6 +100,22 @@
   </si>
   <si>
     <t>DateTimeCol05</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>**comment**</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaaa</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bbb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ccc</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -478,15 +494,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -496,8 +515,11 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -507,8 +529,11 @@
       <c r="C2">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -518,8 +543,11 @@
       <c r="C3">
         <v>99</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -528,6 +556,9 @@
       </c>
       <c r="C4">
         <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -709,7 +740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Skip empty data when reading
</commit_message>
<xml_diff>
--- a/src/SSDTHelperTest/TestData.xlsx
+++ b/src/SSDTHelperTest/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="People" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="DataTypeAndFormatPattern" sheetId="5" r:id="rId3"/>
     <sheet name="NullValue" sheetId="6" r:id="rId4"/>
     <sheet name="ResultCheckSheet" sheetId="4" r:id="rId5"/>
+    <sheet name="BlankRow" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t>Age</t>
     <phoneticPr fontId="1"/>
@@ -129,6 +130,22 @@
   </si>
   <si>
     <t>VarCharCol01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Fuga</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FugaFuga</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -162,12 +179,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -182,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -193,6 +216,7 @@
     <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -510,7 +534,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -753,7 +777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -816,9 +840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -924,4 +946,63 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix compare date type problem
</commit_message>
<xml_diff>
--- a/src/SSDTHelperTest/TestData.xlsx
+++ b/src/SSDTHelperTest/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="People" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,8 @@
     <sheet name="DataTypeAndFormatPattern" sheetId="5" r:id="rId3"/>
     <sheet name="NullValue" sheetId="6" r:id="rId4"/>
     <sheet name="ResultCheckSheet" sheetId="4" r:id="rId5"/>
-    <sheet name="BlankRow" sheetId="7" r:id="rId6"/>
+    <sheet name="ResultCheckSheet2" sheetId="8" r:id="rId6"/>
+    <sheet name="BlankRow" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="32">
   <si>
     <t>Age</t>
     <phoneticPr fontId="1"/>
@@ -950,9 +951,121 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="3.08203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="18.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.58203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="11.58203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>42736</v>
+      </c>
+      <c r="C2" s="5">
+        <v>42736</v>
+      </c>
+      <c r="D2" s="8">
+        <v>42736</v>
+      </c>
+      <c r="E2" s="8">
+        <v>43100.666666666664</v>
+      </c>
+      <c r="F2" s="8">
+        <v>43100.666666666664</v>
+      </c>
+      <c r="G2" s="8">
+        <v>43100.042372685188</v>
+      </c>
+      <c r="H2" s="8">
+        <v>43100</v>
+      </c>
+      <c r="I2" s="4">
+        <v>9999999.9900000002</v>
+      </c>
+      <c r="J2" s="4">
+        <v>9999999.9000000004</v>
+      </c>
+      <c r="K2" s="4">
+        <v>9999999</v>
+      </c>
+      <c r="L2" s="4">
+        <v>9999999</v>
+      </c>
+      <c r="M2" s="9">
+        <v>9999999</v>
+      </c>
+      <c r="N2" s="9">
+        <v>9999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>

</xml_diff>

<commit_message>
Calculate when reading excel files
</commit_message>
<xml_diff>
--- a/src/SSDTHelperTest/TestData.xlsx
+++ b/src/SSDTHelperTest/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="People" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="ResultCheckSheet" sheetId="4" r:id="rId5"/>
     <sheet name="ResultCheckSheet2" sheetId="8" r:id="rId6"/>
     <sheet name="BlankRow" sheetId="7" r:id="rId7"/>
+    <sheet name="EvaluateFormula" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
   <si>
     <t>Age</t>
     <phoneticPr fontId="1"/>
@@ -147,6 +148,22 @@
   </si>
   <si>
     <t>FugaFuga</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Today</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Year</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Day</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Month</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -953,7 +970,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1118,4 +1137,54 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1">
+        <f ca="1">TODAY()</f>
+        <v>42857</v>
+      </c>
+      <c r="B2">
+        <f ca="1">YEAR(A2)</f>
+        <v>2017</v>
+      </c>
+      <c r="C2">
+        <f ca="1">MONTH(A2)</f>
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <f ca="1">DAY(A2)</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>